<commit_message>
Added count data from 10/18-10/19
</commit_message>
<xml_diff>
--- a/TAD1_temp_trial.xlsx
+++ b/TAD1_temp_trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\Box Sync\Krasileva_Lab\Research\chandler\Krasileva Lab\E9\e9\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyangzhang/Desktop/deaminase/deaminase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{631D593A-ABD0-447A-9FA3-71FD5E8D7055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1008FE2D-C94F-0D4B-A65E-793D3144E4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29800" windowHeight="17940" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
   <si>
     <t>date_counted</t>
   </si>
@@ -72,13 +72,31 @@
   </si>
   <si>
     <t xml:space="preserve">temperature </t>
+  </si>
+  <si>
+    <t>TAD1</t>
+  </si>
+  <si>
+    <t>TAD1 C184A</t>
+  </si>
+  <si>
+    <t>LZ</t>
+  </si>
+  <si>
+    <t>bl21_de3_delta_ung</t>
+  </si>
+  <si>
+    <t>LB_CAM_KAN</t>
+  </si>
+  <si>
+    <t>LB_RIF_CAM_KAN</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +108,27 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,16 +148,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{47EC85B9-D102-414B-8D34-D71B74815AFC}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -430,21 +474,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CA60C-3040-4746-B03B-AB2935AC05B4}">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.83203125" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="6" max="6" width="14.77734375" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" customWidth="1"/>
+    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -482,7 +532,470 @@
         <v>9</v>
       </c>
     </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J2">
+        <v>151</v>
+      </c>
+      <c r="K2">
+        <f>J2/I2</f>
+        <v>3020000000</v>
+      </c>
+      <c r="L2">
+        <f>K8/K2</f>
+        <v>1.162251655629139E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3">
+        <v>28</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I7" si="0">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J3">
+        <v>255</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="1">J3/I3</f>
+        <v>5100000000</v>
+      </c>
+      <c r="L3">
+        <f>K9/K3</f>
+        <v>4.0196078431372548E-8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J4">
+        <v>361</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>7220000000</v>
+      </c>
+      <c r="L4">
+        <f>K10/K4</f>
+        <v>2.7423822714681439E-8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J5">
+        <v>372</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>7440000000</v>
+      </c>
+      <c r="L5">
+        <f>K11/K5</f>
+        <v>4.7446236559139785E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6">
+        <v>28</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J6">
+        <v>245</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>4900000000</v>
+      </c>
+      <c r="L6">
+        <f>K12/K6</f>
+        <v>5.1632653061224489E-8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="3">
+        <v>10282023</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>37</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="J7">
+        <v>155</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>3100000000</v>
+      </c>
+      <c r="L7">
+        <f>K13/K7</f>
+        <v>5.9032258064516129E-8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>351</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9">
+        <v>28</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>205</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>205</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10">
+        <v>37</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>198</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11">
+        <v>23</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>353</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12">
+        <v>28</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>253</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="3">
+        <v>10192023</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13">
+        <v>37</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>183</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
"add data and update plotting"
</commit_message>
<xml_diff>
--- a/TAD1_temp_trial.xlsx
+++ b/TAD1_temp_trial.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyangzhang/Desktop/deaminase/deaminase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1008FE2D-C94F-0D4B-A65E-793D3144E4E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EEE930-5523-904D-989E-3589F76971ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29800" windowHeight="17940" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
+    <workbookView xWindow="8580" yWindow="760" windowWidth="21220" windowHeight="17780" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>CFU</t>
   </si>
   <si>
-    <t>mut freq</t>
-  </si>
-  <si>
     <t>scientist</t>
   </si>
   <si>
@@ -77,9 +74,6 @@
     <t>TAD1</t>
   </si>
   <si>
-    <t>TAD1 C184A</t>
-  </si>
-  <si>
     <t>LZ</t>
   </si>
   <si>
@@ -90,6 +84,12 @@
   </si>
   <si>
     <t>LB_RIF_CAM_KAN</t>
+  </si>
+  <si>
+    <t>TAD1_C184A</t>
+  </si>
+  <si>
+    <t>mut_freq</t>
   </si>
 </sst>
 </file>
@@ -476,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CA60C-3040-4746-B03B-AB2935AC05B4}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -496,7 +496,7 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -511,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -529,24 +529,24 @@
         <v>8</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3">
         <v>10282023</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>23</v>
@@ -569,25 +569,25 @@
         <v>3020000000</v>
       </c>
       <c r="L2">
-        <f>K8/K2</f>
+        <f t="shared" ref="L2:L7" si="0">K8/K2</f>
         <v>1.162251655629139E-7</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>10282023</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F3">
         <v>28</v>
@@ -599,36 +599,36 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="0">10^-6*0.05</f>
+        <f t="shared" ref="I3:I7" si="1">10^-6*0.05</f>
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J3">
         <v>255</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K13" si="1">J3/I3</f>
+        <f t="shared" ref="K3:K13" si="2">J3/I3</f>
         <v>5100000000</v>
       </c>
       <c r="L3">
-        <f>K9/K3</f>
+        <f t="shared" si="0"/>
         <v>4.0196078431372548E-8</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3">
         <v>10282023</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F4">
         <v>37</v>
@@ -640,36 +640,36 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J4">
         <v>361</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7220000000</v>
       </c>
       <c r="L4">
-        <f>K10/K4</f>
+        <f t="shared" si="0"/>
         <v>2.7423822714681439E-8</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="3">
         <v>10282023</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="C5" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F5">
         <v>23</v>
@@ -681,36 +681,36 @@
         <v>1</v>
       </c>
       <c r="I5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J5">
         <v>372</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7440000000</v>
       </c>
       <c r="L5">
-        <f>K11/K5</f>
+        <f t="shared" si="0"/>
         <v>4.7446236559139785E-8</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3">
         <v>10282023</v>
       </c>
-      <c r="C6" t="s">
-        <v>13</v>
+      <c r="C6" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F6">
         <v>28</v>
@@ -722,36 +722,36 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J6">
         <v>245</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4900000000</v>
       </c>
       <c r="L6">
-        <f>K12/K6</f>
+        <f t="shared" si="0"/>
         <v>5.1632653061224489E-8</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="3">
         <v>10282023</v>
       </c>
-      <c r="C7" t="s">
-        <v>13</v>
+      <c r="C7" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F7">
         <v>37</v>
@@ -763,36 +763,36 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
       <c r="J7">
         <v>155</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3100000000</v>
       </c>
       <c r="L7">
-        <f>K13/K7</f>
+        <f t="shared" si="0"/>
         <v>5.9032258064516129E-8</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>10192023</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F8">
         <v>23</v>
@@ -810,25 +810,25 @@
         <v>351</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>351</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3">
         <v>10192023</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F9">
         <v>28</v>
@@ -846,25 +846,25 @@
         <v>205</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>205</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3">
         <v>10192023</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F10">
         <v>37</v>
@@ -882,25 +882,25 @@
         <v>198</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>198</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="3">
         <v>10192023</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F11">
         <v>23</v>
@@ -918,25 +918,25 @@
         <v>353</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B12" s="3">
         <v>10192023</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F12">
         <v>28</v>
@@ -954,25 +954,25 @@
         <v>253</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B13" s="3">
         <v>10192023</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="F13">
         <v>37</v>
@@ -990,7 +990,7 @@
         <v>183</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>183</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data sharing with counts
</commit_message>
<xml_diff>
--- a/TAD1_temp_trial.xlsx
+++ b/TAD1_temp_trial.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyangzhang/Desktop/deaminase/deaminase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86EEE930-5523-904D-989E-3589F76971ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A00093A-319D-FF46-8041-F9B37D5F6665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8580" yWindow="760" windowWidth="21220" windowHeight="17780" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
+    <workbookView xWindow="3880" yWindow="760" windowWidth="25920" windowHeight="15760" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="21">
   <si>
     <t>date_counted</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t>mut_freq</t>
+  </si>
+  <si>
+    <t>iptg</t>
+  </si>
+  <si>
+    <t>induction</t>
+  </si>
+  <si>
+    <t>HsAID</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CA60C-3040-4746-B03B-AB2935AC05B4}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="107" workbookViewId="0">
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,14 +496,15 @@
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="5" max="5" width="15.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="7" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" customWidth="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -511,28 +521,35 @@
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -548,32 +565,32 @@
       <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2">
-        <v>23</v>
-      </c>
       <c r="G2">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
         <f>10^-6*0.05</f>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>151</v>
       </c>
-      <c r="K2">
-        <f>J2/I2</f>
+      <c r="M2">
+        <f>L2/K2</f>
         <v>3020000000</v>
       </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L7" si="0">K8/K2</f>
+      <c r="N2">
+        <f t="shared" ref="N2:N7" si="0">M8/M2</f>
         <v>1.162251655629139E-7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -589,32 +606,32 @@
       <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>28</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I7" si="1">10^-6*0.05</f>
+        <v>1</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K7" si="1">10^-6*0.05</f>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>255</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K13" si="2">J3/I3</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M13" si="2">L3/K3</f>
         <v>5100000000</v>
       </c>
-      <c r="L3">
+      <c r="N3">
         <f t="shared" si="0"/>
         <v>4.0196078431372548E-8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -630,32 +647,32 @@
       <c r="E4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>37</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
       <c r="H4">
         <v>1</v>
       </c>
       <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="K4">
         <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>361</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <f t="shared" si="2"/>
         <v>7220000000</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <f t="shared" si="0"/>
         <v>2.7423822714681439E-8</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -671,32 +688,32 @@
       <c r="E5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
-        <v>23</v>
-      </c>
       <c r="G5">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
       <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
         <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>372</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <f t="shared" si="2"/>
         <v>7440000000</v>
       </c>
-      <c r="L5">
+      <c r="N5">
         <f t="shared" si="0"/>
         <v>4.7446236559139785E-8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -712,32 +729,32 @@
       <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>28</v>
       </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
       <c r="H6">
         <v>1</v>
       </c>
       <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>245</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <f t="shared" si="2"/>
         <v>4900000000</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>5.1632653061224489E-8</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -753,32 +770,32 @@
       <c r="E7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>37</v>
       </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
       <c r="H7">
         <v>1</v>
       </c>
       <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
         <f t="shared" si="1"/>
         <v>4.9999999999999998E-8</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>155</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <f t="shared" si="2"/>
         <v>3100000000</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>5.9032258064516129E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -794,11 +811,8 @@
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F8">
-        <v>23</v>
-      </c>
       <c r="G8">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -806,15 +820,18 @@
       <c r="I8">
         <v>1</v>
       </c>
-      <c r="J8">
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8">
         <v>351</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <f t="shared" si="2"/>
         <v>351</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -830,27 +847,27 @@
       <c r="E9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>28</v>
       </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
       <c r="H9">
         <v>1</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9">
+      <c r="K9">
+        <v>1</v>
+      </c>
+      <c r="L9">
         <v>205</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <f t="shared" si="2"/>
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -866,27 +883,27 @@
       <c r="E10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>37</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10">
         <v>198</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <f t="shared" si="2"/>
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -902,11 +919,8 @@
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F11">
-        <v>23</v>
-      </c>
       <c r="G11">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -914,15 +928,18 @@
       <c r="I11">
         <v>1</v>
       </c>
-      <c r="J11">
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11">
         <v>353</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <f t="shared" si="2"/>
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -938,27 +955,27 @@
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>28</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
       <c r="H12">
         <v>1</v>
       </c>
       <c r="I12">
         <v>1</v>
       </c>
-      <c r="J12">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
         <v>253</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <f t="shared" si="2"/>
         <v>253</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -974,25 +991,949 @@
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>37</v>
       </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
       <c r="H13">
         <v>1</v>
       </c>
       <c r="I13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
         <v>183</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>23</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ref="K14:K17" si="3">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L14">
+        <v>307</v>
+      </c>
+      <c r="M14">
+        <f>L14/K14</f>
+        <v>6140000000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>23</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L15">
+        <v>333</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ref="M15:M19" si="4">L15/K15</f>
+        <v>6660000000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16">
+        <v>23</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L16">
+        <v>300</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="4"/>
+        <v>6000000000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>23</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="3"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L17">
+        <v>465</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="4"/>
+        <v>9300000000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18">
+        <v>23</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>759</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="4"/>
+        <v>759</v>
+      </c>
+      <c r="N18">
+        <f>M18/M14</f>
+        <v>1.2361563517915309E-7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="3">
+        <v>10292023</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19">
+        <v>23</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>908</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="4"/>
+        <v>908</v>
+      </c>
+      <c r="N19">
+        <f>M19/M15</f>
+        <v>1.3633633633633633E-7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="3">
+        <v>45321</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <v>23</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>1333</v>
+      </c>
+      <c r="M20">
+        <f>L20/K20</f>
+        <v>1333</v>
+      </c>
+      <c r="N20">
+        <f>M20/M21</f>
+        <v>1.7679045092838197E-7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="3">
+        <v>45321</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>23</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ref="K21:K23" si="5">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L21">
+        <v>377</v>
+      </c>
+      <c r="M21">
+        <f>L21/K21</f>
+        <v>7540000000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>23</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="5"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L22">
+        <v>309</v>
+      </c>
+      <c r="M22">
+        <f>L22/K22</f>
+        <v>6180000000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>23</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="5"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L23">
+        <v>315</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ref="M23:M27" si="6">L23/K23</f>
+        <v>6300000000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>13</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G24">
+        <v>23</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ref="K24" si="7">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L24">
+        <v>314</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="6"/>
+        <v>6280000000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>13</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>23</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="K25">
+        <v>0.1</v>
+      </c>
+      <c r="L25">
+        <v>970</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="6"/>
+        <v>9700</v>
+      </c>
+      <c r="N25">
+        <f>M25/M22</f>
+        <v>1.56957928802589E-6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" t="s">
+        <v>13</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26">
+        <v>23</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>490</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="6"/>
+        <v>490</v>
+      </c>
+      <c r="N26">
+        <f>M26/M23</f>
+        <v>7.7777777777777782E-8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" t="s">
+        <v>13</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27">
+        <v>23</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>365</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="6"/>
+        <v>365</v>
+      </c>
+      <c r="N27">
+        <f>M27/M24</f>
+        <v>5.8121019108280256E-8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28">
+        <v>23</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ref="K28" si="8">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L28">
+        <v>391</v>
+      </c>
+      <c r="M28">
+        <f>L28/K28</f>
+        <v>7820000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29">
+        <v>23</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ref="K29:K32" si="9">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L29">
+        <v>285</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ref="M29:M37" si="10">L29/K29</f>
+        <v>5700000000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G30">
+        <v>23</v>
+      </c>
+      <c r="H30">
+        <v>2</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="9"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L30">
+        <v>345</v>
+      </c>
+      <c r="M30">
+        <f t="shared" si="10"/>
+        <v>6900000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>12</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G31">
+        <v>23</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
+      </c>
+      <c r="K31">
+        <f t="shared" si="9"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L31">
+        <v>407</v>
+      </c>
+      <c r="M31">
+        <f t="shared" si="10"/>
+        <v>8140000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32">
+        <v>23</v>
+      </c>
+      <c r="H32">
+        <v>2</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="K32">
+        <f t="shared" si="9"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L32">
+        <v>424</v>
+      </c>
+      <c r="M32">
+        <f t="shared" si="10"/>
+        <v>8480000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33">
+        <v>23</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>1</v>
+      </c>
+      <c r="K33">
+        <v>0.1</v>
+      </c>
+      <c r="L33">
+        <v>872</v>
+      </c>
+      <c r="M33">
+        <f t="shared" si="10"/>
+        <v>8720</v>
+      </c>
+      <c r="N33">
+        <f>M33/M28</f>
+        <v>1.1150895140664961E-6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>12</v>
+      </c>
+      <c r="B34" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34">
+        <v>23</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>1</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34">
+        <v>370</v>
+      </c>
+      <c r="M34">
+        <f t="shared" si="10"/>
+        <v>370</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:N37" si="11">M34/M29</f>
+        <v>6.4912280701754385E-8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35">
+        <v>23</v>
+      </c>
+      <c r="H35">
+        <v>2</v>
+      </c>
+      <c r="I35">
+        <v>1</v>
+      </c>
+      <c r="K35">
+        <v>1</v>
+      </c>
+      <c r="L35">
+        <v>435</v>
+      </c>
+      <c r="M35">
+        <f t="shared" si="10"/>
+        <v>435</v>
+      </c>
+      <c r="N35">
+        <f t="shared" si="11"/>
+        <v>6.3043478260869569E-8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36">
+        <v>23</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="K36">
+        <v>1</v>
+      </c>
+      <c r="L36">
+        <v>424</v>
+      </c>
+      <c r="M36">
+        <f t="shared" si="10"/>
+        <v>424</v>
+      </c>
+      <c r="N36">
+        <f t="shared" si="11"/>
+        <v>5.2088452088452085E-8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37">
+        <v>23</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>1</v>
+      </c>
+      <c r="K37">
+        <v>1</v>
+      </c>
+      <c r="L37">
+        <v>520</v>
+      </c>
+      <c r="M37">
+        <f t="shared" si="10"/>
+        <v>520</v>
+      </c>
+      <c r="N37">
+        <f t="shared" si="11"/>
+        <v>6.1320754716981128E-8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B38" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
other candidates at 23C
</commit_message>
<xml_diff>
--- a/TAD1_temp_trial.xlsx
+++ b/TAD1_temp_trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyangzhang/Desktop/deaminase/deaminase/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A00093A-319D-FF46-8041-F9B37D5F6665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D2823D-963E-6B4C-99C6-400D66F367C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3880" yWindow="760" windowWidth="25920" windowHeight="15760" xr2:uid="{65ADB98C-3120-4740-BD85-DA96AEEF478F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="32">
   <si>
     <t>date_counted</t>
   </si>
@@ -99,6 +99,39 @@
   </si>
   <si>
     <t>HsAID</t>
+  </si>
+  <si>
+    <t>CDA1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>CDAL7</t>
+  </si>
+  <si>
+    <t>PyrD</t>
+  </si>
+  <si>
+    <t>GsDA</t>
+  </si>
+  <si>
+    <t>CDAL4</t>
+  </si>
+  <si>
+    <t>TAD3</t>
+  </si>
+  <si>
+    <t>CDAL1</t>
+  </si>
+  <si>
+    <t>CDAL2</t>
+  </si>
+  <si>
+    <t>CDAL5</t>
+  </si>
+  <si>
+    <t>CDAL6</t>
   </si>
 </sst>
 </file>
@@ -483,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C7CA60C-3040-4746-B03B-AB2935AC05B4}">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="107" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="57" workbookViewId="0">
+      <selection activeCell="K56" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1924,16 +1957,860 @@
         <v>520</v>
       </c>
       <c r="M37">
-        <f t="shared" si="10"/>
+        <f>L37/K37</f>
         <v>520</v>
       </c>
       <c r="N37">
-        <f t="shared" si="11"/>
+        <f>M37/M32</f>
         <v>6.1320754716981128E-8</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="3"/>
+      <c r="A38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B38" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38">
+        <v>23</v>
+      </c>
+      <c r="H38">
+        <v>1</v>
+      </c>
+      <c r="I38">
+        <v>1</v>
+      </c>
+      <c r="K38">
+        <f t="shared" ref="K38:K48" si="12">10^-6*0.05</f>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L38">
+        <v>420</v>
+      </c>
+      <c r="M38">
+        <f>L38/K38</f>
+        <v>8400000000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B39" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G39">
+        <v>23</v>
+      </c>
+      <c r="H39">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>1</v>
+      </c>
+      <c r="K39">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L39">
+        <v>295</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ref="M39:M59" si="13">L39/K39</f>
+        <v>5900000000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G40">
+        <v>23</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <v>1</v>
+      </c>
+      <c r="K40">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L40">
+        <v>305</v>
+      </c>
+      <c r="M40">
+        <f t="shared" si="13"/>
+        <v>6100000000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>12</v>
+      </c>
+      <c r="B41" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G41">
+        <v>23</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+      <c r="I41">
+        <v>1</v>
+      </c>
+      <c r="K41">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L41">
+        <v>341</v>
+      </c>
+      <c r="M41">
+        <f t="shared" si="13"/>
+        <v>6820000000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>12</v>
+      </c>
+      <c r="B42" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D42" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G42">
+        <v>23</v>
+      </c>
+      <c r="H42">
+        <v>1</v>
+      </c>
+      <c r="I42">
+        <v>1</v>
+      </c>
+      <c r="K42">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L42">
+        <v>287</v>
+      </c>
+      <c r="M42">
+        <f t="shared" si="13"/>
+        <v>5740000000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>12</v>
+      </c>
+      <c r="B43" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+      <c r="I43">
+        <v>1</v>
+      </c>
+      <c r="K43">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L43">
+        <v>449</v>
+      </c>
+      <c r="M43">
+        <f t="shared" si="13"/>
+        <v>8980000000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44">
+        <v>23</v>
+      </c>
+      <c r="H44">
+        <v>1</v>
+      </c>
+      <c r="I44">
+        <v>1</v>
+      </c>
+      <c r="K44">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L44">
+        <v>327</v>
+      </c>
+      <c r="M44">
+        <f t="shared" si="13"/>
+        <v>6540000000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G45">
+        <v>23</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+      <c r="I45">
+        <v>1</v>
+      </c>
+      <c r="K45">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L45">
+        <v>297</v>
+      </c>
+      <c r="M45">
+        <f t="shared" si="13"/>
+        <v>5940000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G46">
+        <v>23</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+      <c r="I46">
+        <v>1</v>
+      </c>
+      <c r="K46">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L46">
+        <v>372</v>
+      </c>
+      <c r="M46">
+        <f t="shared" si="13"/>
+        <v>7440000000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>12</v>
+      </c>
+      <c r="B47" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G47">
+        <v>23</v>
+      </c>
+      <c r="H47">
+        <v>1</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L47">
+        <v>404</v>
+      </c>
+      <c r="M47">
+        <f t="shared" si="13"/>
+        <v>8080000000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>12</v>
+      </c>
+      <c r="B48" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G48">
+        <v>23</v>
+      </c>
+      <c r="H48">
+        <v>1</v>
+      </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="K48">
+        <f t="shared" si="12"/>
+        <v>4.9999999999999998E-8</v>
+      </c>
+      <c r="L48">
+        <v>239</v>
+      </c>
+      <c r="M48">
+        <f t="shared" si="13"/>
+        <v>4780000000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D49" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49">
+        <v>23</v>
+      </c>
+      <c r="H49">
+        <v>1</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49">
+        <v>382</v>
+      </c>
+      <c r="M49">
+        <f t="shared" si="13"/>
+        <v>382</v>
+      </c>
+      <c r="N49">
+        <f>M49/M38</f>
+        <v>4.5476190476190479E-8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>12</v>
+      </c>
+      <c r="B50" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D50" t="s">
+        <v>13</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50">
+        <v>23</v>
+      </c>
+      <c r="H50">
+        <v>1</v>
+      </c>
+      <c r="I50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>380</v>
+      </c>
+      <c r="M50">
+        <f t="shared" si="13"/>
+        <v>380</v>
+      </c>
+      <c r="N50">
+        <f t="shared" ref="N50:N59" si="14">M50/M39</f>
+        <v>6.440677966101695E-8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>12</v>
+      </c>
+      <c r="B51" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D51" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51">
+        <v>23</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>1</v>
+      </c>
+      <c r="K51">
+        <v>1</v>
+      </c>
+      <c r="L51">
+        <v>344</v>
+      </c>
+      <c r="M51">
+        <f t="shared" si="13"/>
+        <v>344</v>
+      </c>
+      <c r="N51">
+        <f t="shared" si="14"/>
+        <v>5.6393442622950821E-8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>12</v>
+      </c>
+      <c r="B52" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52">
+        <v>23</v>
+      </c>
+      <c r="H52">
+        <v>1</v>
+      </c>
+      <c r="I52">
+        <v>1</v>
+      </c>
+      <c r="K52">
+        <v>1</v>
+      </c>
+      <c r="L52">
+        <v>504</v>
+      </c>
+      <c r="M52">
+        <f t="shared" si="13"/>
+        <v>504</v>
+      </c>
+      <c r="N52">
+        <f t="shared" si="14"/>
+        <v>7.3900293255131959E-8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>12</v>
+      </c>
+      <c r="B53" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G53">
+        <v>23</v>
+      </c>
+      <c r="H53">
+        <v>1</v>
+      </c>
+      <c r="I53">
+        <v>1</v>
+      </c>
+      <c r="K53">
+        <v>1</v>
+      </c>
+      <c r="L53">
+        <v>346</v>
+      </c>
+      <c r="M53">
+        <f t="shared" si="13"/>
+        <v>346</v>
+      </c>
+      <c r="N53">
+        <f t="shared" si="14"/>
+        <v>6.0278745644599307E-8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>12</v>
+      </c>
+      <c r="B54" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54">
+        <v>23</v>
+      </c>
+      <c r="H54">
+        <v>1</v>
+      </c>
+      <c r="I54">
+        <v>1</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54">
+        <v>482</v>
+      </c>
+      <c r="M54">
+        <f t="shared" si="13"/>
+        <v>482</v>
+      </c>
+      <c r="N54">
+        <f t="shared" si="14"/>
+        <v>5.3674832962138083E-8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55">
+        <v>23</v>
+      </c>
+      <c r="H55">
+        <v>1</v>
+      </c>
+      <c r="I55">
+        <v>1</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55">
+        <v>509</v>
+      </c>
+      <c r="M55">
+        <f t="shared" si="13"/>
+        <v>509</v>
+      </c>
+      <c r="N55">
+        <f t="shared" si="14"/>
+        <v>7.7828746177370029E-8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56">
+        <v>23</v>
+      </c>
+      <c r="H56">
+        <v>1</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56">
+        <v>485</v>
+      </c>
+      <c r="M56">
+        <f t="shared" si="13"/>
+        <v>485</v>
+      </c>
+      <c r="N56">
+        <f t="shared" si="14"/>
+        <v>8.1649831649831649E-8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D57" t="s">
+        <v>13</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57">
+        <v>23</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="K57">
+        <v>1</v>
+      </c>
+      <c r="L57">
+        <v>840</v>
+      </c>
+      <c r="M57">
+        <f t="shared" si="13"/>
+        <v>840</v>
+      </c>
+      <c r="N57">
+        <f t="shared" si="14"/>
+        <v>1.1290322580645161E-7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>12</v>
+      </c>
+      <c r="B58" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D58" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58">
+        <v>23</v>
+      </c>
+      <c r="H58">
+        <v>1</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>1</v>
+      </c>
+      <c r="L58">
+        <v>609</v>
+      </c>
+      <c r="M58">
+        <f t="shared" si="13"/>
+        <v>609</v>
+      </c>
+      <c r="N58">
+        <f t="shared" si="14"/>
+        <v>7.5371287128712866E-8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>12</v>
+      </c>
+      <c r="B59" s="3">
+        <v>45370</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D59" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59">
+        <v>23</v>
+      </c>
+      <c r="H59">
+        <v>1</v>
+      </c>
+      <c r="I59">
+        <v>1</v>
+      </c>
+      <c r="K59">
+        <v>1</v>
+      </c>
+      <c r="L59">
+        <v>468</v>
+      </c>
+      <c r="M59">
+        <f t="shared" si="13"/>
+        <v>468</v>
+      </c>
+      <c r="N59">
+        <f t="shared" si="14"/>
+        <v>9.7907949790794981E-8</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>